<commit_message>
Update Oversigt over mangle rapport.xlsx
</commit_message>
<xml_diff>
--- a/Oversigt over mangle rapport.xlsx
+++ b/Oversigt over mangle rapport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24805"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\OneDrive\Skrivebord\CityCrawl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{434C746F-37BB-4487-8F4E-1D93D4103B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D9F380-A6AB-48A3-BBE2-BA5ADE782698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="3040" windowWidth="16920" windowHeight="10460" xr2:uid="{467DCD83-1D97-4EFF-A296-8E75A6D29487}"/>
   </bookViews>
@@ -163,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -545,19 +545,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58337C14-DA5B-4B04-8DE1-CDE8F1182865}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,177 +577,177 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>40</v>
       </c>

</xml_diff>